<commit_message>
misc changes for submission
</commit_message>
<xml_diff>
--- a/discussion/biplot-packages.xlsx
+++ b/discussion/biplot-packages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\R\projects\ggbiplot\discussion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A597ED12-DC5C-43DD-A610-E3B6E0808A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648A6124-EEAE-4DA0-8888-6BE22487D1B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="96" yWindow="696" windowWidth="20064" windowHeight="11304" xr2:uid="{9C5127FA-2402-488A-ABC9-F429EC7F5995}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>package</t>
   </si>
@@ -117,6 +117,12 @@
   </si>
   <si>
     <t>How to Create a Biplot in R</t>
+  </si>
+  <si>
+    <t>pcaMethods</t>
+  </si>
+  <si>
+    <t>The pcaMethods Package</t>
   </si>
 </sst>
 </file>
@@ -482,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55816383-A54F-4316-A729-FDE73AFBB1C2}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -549,6 +555,9 @@
       <c r="D5" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -614,6 +623,17 @@
       </c>
       <c r="E11" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -631,8 +651,10 @@
     <hyperlink ref="E10" r:id="rId11" xr:uid="{3DEB7BC4-FF0F-406B-85DC-7D5296B66438}"/>
     <hyperlink ref="E6" r:id="rId12" xr:uid="{DCC2419B-EB85-4590-9AB8-CEFC80082310}"/>
     <hyperlink ref="E3" r:id="rId13" xr:uid="{252378F2-869B-4080-91FD-A60BC7CF2988}"/>
+    <hyperlink ref="A12" r:id="rId14" xr:uid="{3DBD22E2-59A8-4151-AFFD-D2547C5D5A4D}"/>
+    <hyperlink ref="E12" r:id="rId15" xr:uid="{BE5C5EE6-50C3-4A99-91C2-580089CA5CEB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId14"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>